<commit_message>
Arzobispo 4 sept 2025
</commit_message>
<xml_diff>
--- a/FORMACIONES/PROGRAMACION DE SOFTWARE/SEGUIMIENTO/SEGUIMIENTO.xlsx
+++ b/FORMACIONES/PROGRAMACION DE SOFTWARE/SEGUIMIENTO/SEGUIMIENTO.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/34e177e0cbf82b1c/ONE DRIVE COMPARTIDOS PC/SENATEC/FORMACIONES/PROGRAMACIÓN DE SOFTWARE/SEGUIMIENTO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SharkCoder Laptop\Desktop\SENATIC\FORMACIONES\PROGRAMACION DE SOFTWARE\SEGUIMIENTO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="13_ncr:1_{7E4ABA11-D274-4921-B24C-D0A10A4C5C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{058C5B5A-92E7-4168-9D05-A388A9563B21}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A27E0F6-B4BE-42AC-840A-34414B5DAC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="19386" windowHeight="11466" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MAYO" sheetId="10" r:id="rId1"/>
     <sheet name="JUNIO" sheetId="11" r:id="rId2"/>
     <sheet name="JULIO" sheetId="12" r:id="rId3"/>
     <sheet name="AGOSTO" sheetId="13" r:id="rId4"/>
-    <sheet name="CONSOLIDADO" sheetId="14" r:id="rId5"/>
+    <sheet name="SEPTIEMBRE" sheetId="14" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="30">
   <si>
     <t>#</t>
   </si>
@@ -120,22 +120,19 @@
     <t>AGOSTO</t>
   </si>
   <si>
-    <t>MES</t>
+    <t>BETANCUR RESTREPO  SANTIAGO</t>
   </si>
   <si>
-    <t>JUNIO</t>
+    <t>TALLER</t>
   </si>
   <si>
-    <t>SEPTIEMBRE</t>
+    <t>VARIOS</t>
   </si>
   <si>
-    <t>OCTUBRE</t>
+    <t>WEB</t>
   </si>
   <si>
-    <t>NOVIEMBRE</t>
-  </si>
-  <si>
-    <t>BETANCUR RESTREPO  SANTIAGO</t>
+    <t>INTENS 2</t>
   </si>
 </sst>
 </file>
@@ -146,7 +143,7 @@
     <numFmt numFmtId="164" formatCode="00"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,22 +205,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,8 +261,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -592,12 +581,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -704,17 +708,23 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -795,67 +805,15 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <font>
         <b/>
@@ -1287,50 +1245,50 @@
       <selection activeCell="C4" sqref="C4:C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.3984375" customWidth="1"/>
+    <col min="2" max="2" width="29.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.265625" customWidth="1"/>
+    <col min="8" max="8" width="10.86328125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="44" t="s">
+      <c r="B1" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="35" t="s">
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="36" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="47" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" s="40"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="36"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="40"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="46"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="37"/>
+    </row>
+    <row r="3" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="41"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="47"/>
       <c r="D3" s="1">
         <v>21</v>
       </c>
@@ -1343,9 +1301,9 @@
       <c r="G3" s="1">
         <v>30</v>
       </c>
-      <c r="H3" s="37"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3" s="38"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -1373,7 +1331,7 @@
         <v>3.4375</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -1401,7 +1359,7 @@
         <v>4.0625</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -1429,7 +1387,7 @@
         <v>4.375</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -1457,7 +1415,7 @@
         <v>4.375</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -1485,7 +1443,7 @@
         <v>3.4375</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -1513,7 +1471,7 @@
         <v>3.4375</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -1541,7 +1499,7 @@
         <v>4.0625</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -1569,7 +1527,7 @@
         <v>3.4375</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -1597,7 +1555,7 @@
         <v>3.125</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -1625,7 +1583,7 @@
         <v>3.125</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -1653,7 +1611,7 @@
         <v>4.375</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -1681,7 +1639,7 @@
         <v>4.0625</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -1709,7 +1667,7 @@
         <v>3.125</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -1737,7 +1695,7 @@
         <v>4.375</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -1765,7 +1723,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -1793,7 +1751,7 @@
         <v>4.375</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -1848,18 +1806,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:G20">
-    <cfRule type="expression" dxfId="24" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>D4=""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="between">
       <formula>0</formula>
       <formula>0.3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="between">
       <formula>61%</formula>
       <formula>100%</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="between">
       <formula>31%</formula>
       <formula>60%</formula>
     </cfRule>
@@ -1902,50 +1860,50 @@
       <selection activeCell="C4" sqref="C4:C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.3984375" customWidth="1"/>
+    <col min="2" max="2" width="39.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.265625" customWidth="1"/>
+    <col min="8" max="8" width="10.86328125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="44" t="s">
+      <c r="B1" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="35" t="s">
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="36" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="47" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" s="40"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="36"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="40"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="46"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="37"/>
+    </row>
+    <row r="3" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="41"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="47"/>
       <c r="D3" s="1">
         <v>4</v>
       </c>
@@ -1958,14 +1916,14 @@
       <c r="G3" s="1">
         <v>13</v>
       </c>
-      <c r="H3" s="37"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3" s="38"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C4" s="22">
         <f t="shared" ref="C4:C20" si="0">IFERROR(AVERAGE(D4:G4),0%)</f>
@@ -1988,7 +1946,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -2016,7 +1974,7 @@
         <v>3.125</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -2044,7 +2002,7 @@
         <v>4.0625</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -2072,7 +2030,7 @@
         <v>4.6875</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -2100,7 +2058,7 @@
         <v>3.125</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -2128,7 +2086,7 @@
         <v>3.125</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -2156,7 +2114,7 @@
         <v>4.6875</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -2184,7 +2142,7 @@
         <v>3.4375</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -2212,7 +2170,7 @@
         <v>3.125</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -2240,7 +2198,7 @@
         <v>2.8125</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -2268,7 +2226,7 @@
         <v>4.0625</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -2296,7 +2254,7 @@
         <v>3.4375</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -2324,7 +2282,7 @@
         <v>3.4375</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -2352,7 +2310,7 @@
         <v>4.6875</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -2380,7 +2338,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -2408,7 +2366,7 @@
         <v>4.6875</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -2463,18 +2421,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:G20">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="15" priority="1">
       <formula>D4=""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="between">
       <formula>0</formula>
       <formula>0.3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="between">
       <formula>61%</formula>
       <formula>100%</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="between">
       <formula>31%</formula>
       <formula>60%</formula>
     </cfRule>
@@ -2513,60 +2471,60 @@
   </sheetPr>
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C20"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.3984375" customWidth="1"/>
+    <col min="2" max="2" width="29.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.265625" customWidth="1"/>
+    <col min="11" max="11" width="10.86328125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="44" t="s">
+      <c r="B1" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="35" t="s">
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="36" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="47" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" s="40"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="36"/>
-    </row>
-    <row r="3" spans="1:11" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="40"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="46"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="37"/>
+    </row>
+    <row r="3" spans="1:11" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="41"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="47"/>
       <c r="D3" s="1">
         <v>9</v>
       </c>
@@ -2588,9 +2546,9 @@
       <c r="J3" s="1">
         <v>30</v>
       </c>
-      <c r="K3" s="37"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K3" s="38"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -2599,35 +2557,35 @@
       </c>
       <c r="C4" s="22">
         <f t="shared" ref="C4:C20" si="0">IFERROR(AVERAGE(D4:J4),0%)</f>
-        <v>0.9285714285714286</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="D4" s="4">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E4" s="4">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="F4" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G4" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H4" s="4">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="I4" s="4">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="J4" s="4">
         <v>0.5</v>
       </c>
       <c r="K4" s="13">
         <f t="shared" ref="K4:K20" si="1">5*C4</f>
-        <v>4.6428571428571432</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3.2142857142857144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -2664,7 +2622,7 @@
         <v>4.6428571428571432</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -2701,7 +2659,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -2738,7 +2696,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -2775,7 +2733,7 @@
         <v>4.2857142857142856</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -2812,7 +2770,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -2849,7 +2807,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -2886,7 +2844,7 @@
         <v>4.2857142857142856</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -2923,7 +2881,7 @@
         <v>4.1071428571428568</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -2960,7 +2918,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -2997,7 +2955,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -3034,7 +2992,7 @@
         <v>3.9285714285714284</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -3071,7 +3029,7 @@
         <v>3.0357142857142856</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -3108,7 +3066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -3145,7 +3103,7 @@
         <v>4.6428571428571432</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -3182,7 +3140,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="14">
         <v>18</v>
       </c>
@@ -3246,23 +3204,23 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:J20">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>D4=""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="between">
       <formula>0</formula>
       <formula>0.3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="between">
       <formula>61%</formula>
       <formula>100%</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="between">
       <formula>31%</formula>
       <formula>60%</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:J20" xr:uid="{30304D37-AD92-4B7A-A0EE-317B4C157859}">
       <formula1>"0%,25%,50%,75%,100%"</formula1>
     </dataValidation>
@@ -3294,66 +3252,66 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.3984375" customWidth="1"/>
+    <col min="2" max="2" width="29.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.265625" customWidth="1"/>
+    <col min="13" max="13" width="10.86328125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="44" t="s">
+      <c r="B1" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="51" t="s">
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="52" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="54" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A2" s="40"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="52"/>
-    </row>
-    <row r="3" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="45"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="53"/>
+    </row>
+    <row r="3" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="40"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="46"/>
       <c r="D3" s="5">
         <v>1</v>
       </c>
@@ -3381,9 +3339,9 @@
       <c r="L3" s="5">
         <v>9</v>
       </c>
-      <c r="M3" s="52"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M3" s="53"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -3392,7 +3350,7 @@
       </c>
       <c r="C4" s="20">
         <f t="shared" ref="C4:C20" si="0">IFERROR(AVERAGE(D4:L4),0%)</f>
-        <v>1</v>
+        <v>0.625</v>
       </c>
       <c r="D4" s="24">
         <v>1</v>
@@ -3400,19 +3358,27 @@
       <c r="E4" s="24">
         <v>1</v>
       </c>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
+      <c r="F4" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="24">
+        <v>0.25</v>
+      </c>
+      <c r="I4" s="24">
+        <v>0.5</v>
+      </c>
       <c r="J4" s="24"/>
       <c r="K4" s="24"/>
       <c r="L4" s="24"/>
       <c r="M4" s="26">
         <f t="shared" ref="M4:M20" si="1">5*C4</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -3421,7 +3387,7 @@
       </c>
       <c r="C5" s="20">
         <f t="shared" si="0"/>
-        <v>0.9375</v>
+        <v>0.625</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -3433,19 +3399,23 @@
         <v>1</v>
       </c>
       <c r="G5" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="27">
         <f t="shared" si="1"/>
-        <v>4.6875</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -3454,7 +3424,7 @@
       </c>
       <c r="C6" s="20">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -3468,17 +3438,21 @@
       <c r="G6" s="24">
         <v>1</v>
       </c>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
+      <c r="H6" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="I6" s="24">
+        <v>1</v>
+      </c>
       <c r="J6" s="24"/>
       <c r="K6" s="24"/>
       <c r="L6" s="24"/>
       <c r="M6" s="26">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>4.583333333333333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -3487,7 +3461,7 @@
       </c>
       <c r="C7" s="20">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -3495,19 +3469,27 @@
       <c r="E7" s="2">
         <v>1</v>
       </c>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
+      <c r="F7" s="24">
+        <v>0.75</v>
+      </c>
+      <c r="G7" s="24">
+        <v>0.75</v>
+      </c>
+      <c r="H7" s="24">
+        <v>0.25</v>
+      </c>
+      <c r="I7" s="24">
+        <v>0.75</v>
+      </c>
       <c r="J7" s="24"/>
       <c r="K7" s="24"/>
       <c r="L7" s="24"/>
       <c r="M7" s="26">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -3516,7 +3498,7 @@
       </c>
       <c r="C8" s="20">
         <f t="shared" si="0"/>
-        <v>0.875</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="D8" s="2">
         <v>0.75</v>
@@ -3528,19 +3510,23 @@
         <v>1</v>
       </c>
       <c r="G8" s="24">
-        <v>1</v>
-      </c>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
+        <v>0.5</v>
+      </c>
+      <c r="H8" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="24">
+        <v>0.75</v>
+      </c>
       <c r="J8" s="24"/>
       <c r="K8" s="24"/>
       <c r="L8" s="24"/>
       <c r="M8" s="26">
         <f t="shared" si="1"/>
-        <v>4.375</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3.541666666666667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="6">
         <v>7</v>
       </c>
@@ -3549,7 +3535,7 @@
       </c>
       <c r="C9" s="20">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
@@ -3557,19 +3543,27 @@
       <c r="E9" s="2">
         <v>1</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="F9" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="G9" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.5</v>
+      </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="27">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3.541666666666667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -3578,7 +3572,7 @@
       </c>
       <c r="C10" s="20">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="D10" s="24">
         <v>1</v>
@@ -3592,17 +3586,21 @@
       <c r="G10" s="24">
         <v>1</v>
       </c>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
+      <c r="H10" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="I10" s="24">
+        <v>1</v>
+      </c>
       <c r="J10" s="24"/>
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>
       <c r="M10" s="26">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>4.583333333333333</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -3611,7 +3609,7 @@
       </c>
       <c r="C11" s="20">
         <f t="shared" si="0"/>
-        <v>0.9375</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="D11" s="25">
         <v>1</v>
@@ -3623,19 +3621,23 @@
         <v>1</v>
       </c>
       <c r="G11" s="24">
-        <v>0.75</v>
-      </c>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
+        <v>0.5</v>
+      </c>
+      <c r="H11" s="24">
+        <v>0</v>
+      </c>
+      <c r="I11" s="24">
+        <v>0.75</v>
+      </c>
       <c r="J11" s="24"/>
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
       <c r="M11" s="26">
         <f t="shared" si="1"/>
-        <v>4.6875</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3.541666666666667</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -3644,7 +3646,7 @@
       </c>
       <c r="C12" s="20">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
@@ -3656,19 +3658,23 @@
         <v>1</v>
       </c>
       <c r="G12" s="24">
-        <v>1</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.75</v>
+      </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="27">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3.541666666666667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="6">
         <v>11</v>
       </c>
@@ -3677,7 +3683,7 @@
       </c>
       <c r="C13" s="20">
         <f t="shared" si="0"/>
-        <v>0.3125</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="D13" s="24">
         <v>1</v>
@@ -3691,17 +3697,21 @@
       <c r="G13" s="24">
         <v>0</v>
       </c>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
+      <c r="H13" s="24">
+        <v>0</v>
+      </c>
+      <c r="I13" s="24">
+        <v>0</v>
+      </c>
       <c r="J13" s="24"/>
       <c r="K13" s="24"/>
       <c r="L13" s="24"/>
       <c r="M13" s="26">
         <f t="shared" si="1"/>
-        <v>1.5625</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1.0416666666666667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="6">
         <v>12</v>
       </c>
@@ -3721,9 +3731,15 @@
       <c r="F14" s="24">
         <v>1</v>
       </c>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
+      <c r="G14" s="24">
+        <v>1</v>
+      </c>
+      <c r="H14" s="24">
+        <v>1</v>
+      </c>
+      <c r="I14" s="24">
+        <v>1</v>
+      </c>
       <c r="J14" s="24"/>
       <c r="K14" s="24"/>
       <c r="L14" s="24"/>
@@ -3732,7 +3748,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="6">
         <v>13</v>
       </c>
@@ -3741,7 +3757,7 @@
       </c>
       <c r="C15" s="20">
         <f t="shared" si="0"/>
-        <v>0.625</v>
+        <v>0.375</v>
       </c>
       <c r="D15" s="24">
         <v>1</v>
@@ -3749,19 +3765,27 @@
       <c r="E15" s="24">
         <v>0.25</v>
       </c>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
+      <c r="F15" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="H15" s="24">
+        <v>0</v>
+      </c>
+      <c r="I15" s="24">
+        <v>0</v>
+      </c>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
       <c r="L15" s="24"/>
       <c r="M15" s="26">
         <f t="shared" si="1"/>
-        <v>3.125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1.875</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="6">
         <v>14</v>
       </c>
@@ -3770,7 +3794,7 @@
       </c>
       <c r="C16" s="20">
         <f t="shared" si="0"/>
-        <v>0.875</v>
+        <v>0.625</v>
       </c>
       <c r="D16" s="24">
         <v>0.5</v>
@@ -3782,19 +3806,23 @@
         <v>1</v>
       </c>
       <c r="G16" s="24">
-        <v>1</v>
-      </c>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
+        <v>0.5</v>
+      </c>
+      <c r="H16" s="24">
+        <v>0.25</v>
+      </c>
+      <c r="I16" s="24">
+        <v>0.5</v>
+      </c>
       <c r="J16" s="24"/>
       <c r="K16" s="24"/>
       <c r="L16" s="24"/>
       <c r="M16" s="26">
         <f t="shared" si="1"/>
-        <v>4.375</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="6">
         <v>15</v>
       </c>
@@ -3803,7 +3831,7 @@
       </c>
       <c r="C17" s="20">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="D17" s="24">
         <v>1</v>
@@ -3817,17 +3845,21 @@
       <c r="G17" s="24">
         <v>1</v>
       </c>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
+      <c r="H17" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="I17" s="24">
+        <v>1</v>
+      </c>
       <c r="J17" s="24"/>
       <c r="K17" s="24"/>
       <c r="L17" s="24"/>
       <c r="M17" s="26">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <v>4.583333333333333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="6">
         <v>16</v>
       </c>
@@ -3836,7 +3868,7 @@
       </c>
       <c r="C18" s="20">
         <f t="shared" si="0"/>
-        <v>0.9375</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="D18" s="24">
         <v>1</v>
@@ -3850,17 +3882,21 @@
       <c r="G18" s="24">
         <v>0.75</v>
       </c>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
+      <c r="H18" s="24">
+        <v>0</v>
+      </c>
+      <c r="I18" s="24">
+        <v>1</v>
+      </c>
       <c r="J18" s="24"/>
       <c r="K18" s="24"/>
       <c r="L18" s="24"/>
       <c r="M18" s="26">
         <f t="shared" si="1"/>
-        <v>4.6875</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3.958333333333333</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="6">
         <v>17</v>
       </c>
@@ -3869,7 +3905,7 @@
       </c>
       <c r="C19" s="20">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="D19" s="24">
         <v>1</v>
@@ -3883,17 +3919,21 @@
       <c r="G19" s="24">
         <v>1</v>
       </c>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
+      <c r="H19" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="I19" s="24">
+        <v>1</v>
+      </c>
       <c r="J19" s="24"/>
       <c r="K19" s="24"/>
       <c r="L19" s="24"/>
       <c r="M19" s="26">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>4.583333333333333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="7">
         <v>18</v>
       </c>
@@ -3902,7 +3942,7 @@
       </c>
       <c r="C20" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="D20" s="28">
         <v>1</v>
@@ -3910,16 +3950,35 @@
       <c r="E20" s="28">
         <v>1</v>
       </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
+      <c r="F20" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="G20" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="H20" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="I20" s="30">
+        <v>1</v>
+      </c>
       <c r="J20" s="28"/>
       <c r="K20" s="28"/>
       <c r="L20" s="28"/>
       <c r="M20" s="29">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>3.958333333333333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G21" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="H21" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="I21" s="32" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -3946,18 +4005,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:L20">
-    <cfRule type="expression" dxfId="12" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>D4=""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="between">
       <formula>0</formula>
       <formula>0.3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="between">
       <formula>61%</formula>
       <formula>100%</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="between">
       <formula>31%</formula>
       <formula>60%</formula>
     </cfRule>
@@ -3990,598 +4049,550 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D8C348-AA9E-4538-B3EA-237C1FCB1707}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7987CA2B-14DA-4A52-8A0A-C24249E67BBD}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="30" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" style="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="30" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="12" style="30" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="30" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" style="30" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" style="34" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="30"/>
+    <col min="1" max="1" width="5.3984375" customWidth="1"/>
+    <col min="2" max="2" width="29.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.265625" customWidth="1"/>
+    <col min="12" max="12" width="10.86328125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="44" t="s">
+      <c r="B1" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="51" t="s">
+      <c r="D1" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="52" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="55"/>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A2" s="40"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="55" t="s">
+        <v>24</v>
+      </c>
       <c r="E2" s="55"/>
       <c r="F2" s="55"/>
       <c r="G2" s="55"/>
       <c r="H2" s="55"/>
       <c r="I2" s="55"/>
       <c r="J2" s="55"/>
-      <c r="K2" s="52"/>
-    </row>
-    <row r="3" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="5" t="s">
+      <c r="K2" s="55"/>
+      <c r="L2" s="53"/>
+    </row>
+    <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="40"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5">
+        <v>3</v>
+      </c>
+      <c r="G3" s="5">
+        <v>4</v>
+      </c>
+      <c r="H3" s="5">
         <v>5</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" s="52"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I3" s="5">
+        <v>6</v>
+      </c>
+      <c r="J3" s="5">
+        <v>7</v>
+      </c>
+      <c r="K3" s="5">
+        <v>8</v>
+      </c>
+      <c r="L3" s="53"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="22">
-        <f>IFERROR(AVERAGE(D4:G4),0%)</f>
-        <v>0.7053571428571429</v>
+      <c r="C4" s="20">
+        <f t="shared" ref="C4:C20" si="0">IFERROR(AVERAGE(D4:K4),0%)</f>
+        <v>0.5</v>
       </c>
       <c r="D4" s="24">
-        <v>0.6875</v>
-      </c>
-      <c r="E4" s="22">
-        <v>0.5</v>
-      </c>
-      <c r="F4" s="22">
-        <v>0.9285714285714286</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
       <c r="G4" s="24"/>
       <c r="H4" s="24"/>
       <c r="I4" s="24"/>
       <c r="J4" s="24"/>
-      <c r="K4" s="26">
-        <f t="shared" ref="K4:K20" si="0">5*C4</f>
-        <v>3.5267857142857144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K4" s="24"/>
+      <c r="L4" s="26">
+        <f t="shared" ref="L4:L20" si="1">5*C4</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="22">
-        <f t="shared" ref="C5:C20" si="1">IFERROR(AVERAGE(D5:G5),0%)</f>
-        <v>0.78869047619047628</v>
+      <c r="C5" s="20">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D5" s="2">
-        <v>0.8125</v>
-      </c>
-      <c r="E5" s="22">
-        <v>0.625</v>
-      </c>
-      <c r="F5" s="22">
-        <v>0.9285714285714286</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="27">
-        <f t="shared" si="0"/>
-        <v>3.9434523809523814</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K5" s="2"/>
+      <c r="L5" s="27">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="6">
         <v>3</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="22">
-        <f t="shared" si="1"/>
-        <v>0.9375</v>
-      </c>
-      <c r="D6" s="24">
-        <v>0.875</v>
-      </c>
-      <c r="E6" s="22">
-        <v>0.9375</v>
-      </c>
-      <c r="F6" s="22">
-        <v>1</v>
-      </c>
+      <c r="C6" s="20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="24"/>
       <c r="G6" s="24"/>
       <c r="H6" s="24"/>
       <c r="I6" s="24"/>
       <c r="J6" s="24"/>
-      <c r="K6" s="26">
-        <f t="shared" si="0"/>
-        <v>4.6875</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K6" s="24"/>
+      <c r="L6" s="26">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="6">
         <v>4</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="22">
-        <f t="shared" si="1"/>
-        <v>0.89166666666666661</v>
+      <c r="C7" s="20">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D7" s="2">
-        <v>0.875</v>
-      </c>
-      <c r="E7" s="22">
-        <v>0.8</v>
-      </c>
-      <c r="F7" s="22">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="24"/>
       <c r="G7" s="24"/>
       <c r="H7" s="24"/>
       <c r="I7" s="24"/>
       <c r="J7" s="24"/>
-      <c r="K7" s="26">
-        <f t="shared" si="0"/>
-        <v>4.458333333333333</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K7" s="24"/>
+      <c r="L7" s="26">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="6">
         <v>5</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="22">
-        <f t="shared" si="1"/>
-        <v>0.7232142857142857</v>
+      <c r="C8" s="20">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D8" s="2">
-        <v>0.6875</v>
-      </c>
-      <c r="E8" s="22">
-        <v>0.625</v>
-      </c>
-      <c r="F8" s="22">
-        <v>0.8571428571428571</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="24"/>
       <c r="G8" s="24"/>
       <c r="H8" s="24"/>
       <c r="I8" s="24"/>
       <c r="J8" s="24"/>
-      <c r="K8" s="26">
-        <f t="shared" si="0"/>
-        <v>3.6160714285714284</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K8" s="24"/>
+      <c r="L8" s="26">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="6">
         <v>6</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="22">
-        <f t="shared" si="1"/>
-        <v>0.77083333333333337</v>
+      <c r="C9" s="20">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D9" s="2">
-        <v>0.6875</v>
-      </c>
-      <c r="E9" s="22">
-        <v>0.625</v>
-      </c>
-      <c r="F9" s="22">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
       <c r="G9" s="24"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="27">
-        <f t="shared" si="0"/>
-        <v>3.854166666666667</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K9" s="2"/>
+      <c r="L9" s="27">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="6">
         <v>7</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="22">
-        <f t="shared" si="1"/>
-        <v>0.9458333333333333</v>
+      <c r="C10" s="20">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D10" s="24">
-        <v>0.9</v>
-      </c>
-      <c r="E10" s="22">
-        <v>0.9375</v>
-      </c>
-      <c r="F10" s="22">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>
       <c r="I10" s="24"/>
       <c r="J10" s="24"/>
-      <c r="K10" s="26">
-        <f t="shared" si="0"/>
-        <v>4.7291666666666661</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="24"/>
+      <c r="L10" s="26">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="6">
         <v>8</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="22">
-        <f t="shared" si="1"/>
-        <v>0.74404761904761907</v>
+      <c r="C11" s="20">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D11" s="25">
-        <v>0.6875</v>
-      </c>
-      <c r="E11" s="22">
-        <v>0.6875</v>
-      </c>
-      <c r="F11" s="22">
-        <v>0.8571428571428571</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
       <c r="G11" s="24"/>
       <c r="H11" s="24"/>
       <c r="I11" s="24"/>
       <c r="J11" s="24"/>
-      <c r="K11" s="26">
-        <f t="shared" si="0"/>
-        <v>3.7202380952380953</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K11" s="24"/>
+      <c r="L11" s="26">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="6">
         <v>9</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="22">
-        <f t="shared" si="1"/>
-        <v>0.69047619047619035</v>
+      <c r="C12" s="20">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D12" s="2">
-        <v>0.625</v>
-      </c>
-      <c r="E12" s="22">
-        <v>0.625</v>
-      </c>
-      <c r="F12" s="22">
-        <v>0.8214285714285714</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E12" s="24"/>
+      <c r="F12" s="2"/>
       <c r="G12" s="24"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="27">
-        <f t="shared" si="0"/>
-        <v>3.4523809523809517</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K12" s="2"/>
+      <c r="L12" s="27">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="6">
         <v>10</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="22">
-        <f t="shared" si="1"/>
-        <v>0.5625</v>
-      </c>
-      <c r="D13" s="24">
-        <v>0.625</v>
-      </c>
-      <c r="E13" s="22">
-        <v>0.5625</v>
-      </c>
-      <c r="F13" s="22">
-        <v>0.5</v>
-      </c>
+      <c r="C13" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
       <c r="G13" s="24"/>
       <c r="H13" s="24"/>
       <c r="I13" s="24"/>
       <c r="J13" s="24"/>
-      <c r="K13" s="26">
-        <f t="shared" si="0"/>
-        <v>2.8125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K13" s="24"/>
+      <c r="L13" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="6">
         <v>11</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="22">
-        <f t="shared" si="1"/>
-        <v>0.93333333333333324</v>
+      <c r="C14" s="20">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D14" s="24">
-        <v>0.9</v>
-      </c>
-      <c r="E14" s="22">
-        <v>0.9</v>
-      </c>
-      <c r="F14" s="22">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
       <c r="G14" s="24"/>
       <c r="H14" s="24"/>
       <c r="I14" s="24"/>
       <c r="J14" s="24"/>
-      <c r="K14" s="26">
-        <f t="shared" si="0"/>
-        <v>4.6666666666666661</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K14" s="24"/>
+      <c r="L14" s="26">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="6">
         <v>12</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="22">
-        <f t="shared" si="1"/>
-        <v>0.72440476190476188</v>
-      </c>
-      <c r="D15" s="24">
-        <v>0.7</v>
-      </c>
-      <c r="E15" s="22">
-        <v>0.6875</v>
-      </c>
-      <c r="F15" s="22">
-        <v>0.7857142857142857</v>
-      </c>
+      <c r="C15" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
       <c r="G15" s="24"/>
       <c r="H15" s="24"/>
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
-      <c r="K15" s="26">
-        <f t="shared" si="0"/>
-        <v>3.6220238095238093</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K15" s="24"/>
+      <c r="L15" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="6">
         <v>13</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="22">
-        <f t="shared" si="1"/>
-        <v>0.63988095238095244</v>
+      <c r="C16" s="20">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
       </c>
       <c r="D16" s="24">
-        <v>0.625</v>
-      </c>
-      <c r="E16" s="22">
-        <v>0.6875</v>
-      </c>
-      <c r="F16" s="22">
-        <v>0.6071428571428571</v>
-      </c>
+        <v>0.75</v>
+      </c>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
       <c r="G16" s="24"/>
       <c r="H16" s="24"/>
       <c r="I16" s="24"/>
       <c r="J16" s="24"/>
-      <c r="K16" s="26">
-        <f t="shared" si="0"/>
-        <v>3.1994047619047623</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="K16" s="24"/>
+      <c r="L16" s="26">
+        <f t="shared" si="1"/>
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" s="6">
         <v>14</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="22">
-        <f t="shared" si="1"/>
-        <v>0.9375</v>
-      </c>
-      <c r="D17" s="24">
-        <v>0.875</v>
-      </c>
-      <c r="E17" s="22">
-        <v>0.9375</v>
-      </c>
-      <c r="F17" s="22">
-        <v>1</v>
-      </c>
+      <c r="C17" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
       <c r="G17" s="24"/>
       <c r="H17" s="24"/>
       <c r="I17" s="24"/>
       <c r="J17" s="24"/>
-      <c r="K17" s="26">
-        <f t="shared" si="0"/>
-        <v>4.6875</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="24"/>
+      <c r="L17" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" s="6">
         <v>15</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="22">
-        <f t="shared" si="1"/>
-        <v>0.80952380952380965</v>
+      <c r="C18" s="20">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D18" s="24">
-        <v>0.75</v>
-      </c>
-      <c r="E18" s="22">
-        <v>0.75</v>
-      </c>
-      <c r="F18" s="22">
-        <v>0.9285714285714286</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
       <c r="G18" s="24"/>
       <c r="H18" s="24"/>
       <c r="I18" s="24"/>
       <c r="J18" s="24"/>
-      <c r="K18" s="26">
-        <f t="shared" si="0"/>
-        <v>4.0476190476190483</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="24"/>
+      <c r="L18" s="26">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" s="6">
         <v>16</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="22">
-        <f t="shared" si="1"/>
-        <v>0.9375</v>
+      <c r="C19" s="20">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D19" s="24">
-        <v>0.875</v>
-      </c>
-      <c r="E19" s="22">
-        <v>0.9375</v>
-      </c>
-      <c r="F19" s="22">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
       <c r="G19" s="24"/>
       <c r="H19" s="24"/>
       <c r="I19" s="24"/>
       <c r="J19" s="24"/>
-      <c r="K19" s="26">
-        <f t="shared" si="0"/>
-        <v>4.6875</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7">
+      <c r="K19" s="24"/>
+      <c r="L19" s="26">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="6">
         <v>17</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="23">
-        <f t="shared" si="1"/>
-        <v>0.85416666666666663</v>
+      <c r="C20" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D20" s="28">
-        <v>0.75</v>
-      </c>
-      <c r="E20" s="23">
-        <v>0.8125</v>
-      </c>
-      <c r="F20" s="23">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
       <c r="G20" s="28"/>
       <c r="H20" s="28"/>
       <c r="I20" s="28"/>
       <c r="J20" s="28"/>
-      <c r="K20" s="29">
-        <f t="shared" si="0"/>
-        <v>4.270833333333333</v>
-      </c>
+      <c r="K20" s="28"/>
+      <c r="L20" s="29">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="D21" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="33"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C1:C3"/>
-    <mergeCell ref="K1:K3"/>
-    <mergeCell ref="D1:J2"/>
+    <mergeCell ref="D1:K1"/>
+    <mergeCell ref="L1:L3"/>
+    <mergeCell ref="D2:K2"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:C20">
-    <cfRule type="dataBar" priority="17">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4589,119 +4600,40 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{F35CE92F-68CA-4140-BD0F-BE23445072A0}</x14:id>
+          <x14:id>{43DDB61F-6436-49AB-92B2-A42190A82D17}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D20">
-    <cfRule type="expression" dxfId="8" priority="3">
+  <conditionalFormatting sqref="D4:K20">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>D4=""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
       <formula>0</formula>
       <formula>0.3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="between">
       <formula>61%</formula>
       <formula>100%</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="between">
       <formula>31%</formula>
       <formula>60%</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E5 E7:E20">
-    <cfRule type="dataBar" priority="14">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF00B050"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{81498ABC-9826-41EC-95FD-A08D27405480}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="dataBar" priority="2">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF00B050"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{4F973C81-2CCA-47DB-B913-B65B9BEF2905}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F4:F5 F7:F20">
-    <cfRule type="dataBar" priority="13">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF00B050"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{F5BDFC6F-1D47-433B-9035-E2C848310CC3}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F6">
-    <cfRule type="dataBar" priority="1">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF00B050"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3843B687-7674-4D53-8795-3576DB7368AA}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G4:J20">
-    <cfRule type="expression" dxfId="4" priority="19">
-      <formula>G4=""</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="20" operator="between">
-      <formula>0</formula>
-      <formula>0.3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="21" operator="between">
-      <formula>61%</formula>
-      <formula>100%</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="22" operator="between">
-      <formula>31%</formula>
-      <formula>60%</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4:K20">
-    <cfRule type="cellIs" dxfId="0" priority="18" operator="lessThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:J20" xr:uid="{7096D5BB-A5D6-4DC3-AB17-0CAA79390941}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:K20" xr:uid="{A9D697E6-030F-44F3-BC1C-BCE31ED7779C}">
       <formula1>"0%,25%,50%,75%,100%"</formula1>
     </dataValidation>
   </dataValidations>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="122" scale="130" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F35CE92F-68CA-4140-BD0F-BE23445072A0}">
+          <x14:cfRule type="dataBar" id="{43DDB61F-6436-49AB-92B2-A42190A82D17}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -4711,50 +4643,6 @@
           </x14:cfRule>
           <xm:sqref>C4:C20</xm:sqref>
         </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{81498ABC-9826-41EC-95FD-A08D27405480}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E4:E5 E7:E20</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4F973C81-2CCA-47DB-B913-B65B9BEF2905}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E6</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F5BDFC6F-1D47-433B-9035-E2C848310CC3}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>F4:F5 F7:F20</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3843B687-7674-4D53-8795-3576DB7368AA}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>F6</xm:sqref>
-        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>